<commit_message>
Fix dynamic cases and rerun case study
</commit_message>
<xml_diff>
--- a/ACTIVSg200/2.IL200_dyn_20wt_ts.xlsx
+++ b/ACTIVSg200/2.IL200_dyn_20wt_ts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/work/turbinegov/ACTIVSg200/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D802887-435B-8248-AADE-F8EAC67ED4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E43D763-A3A3-E146-9E39-62C05292364E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18880" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1540" windowWidth="34560" windowHeight="19000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1945" uniqueCount="1019">
   <si>
     <t>idx</t>
   </si>
@@ -2516,6 +2516,9 @@
   </si>
   <si>
     <t>IEEEG1_25</t>
+  </si>
+  <si>
+    <t>IEEEG1_26</t>
   </si>
   <si>
     <t>KT</t>
@@ -12330,11 +12333,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:AC26"/>
+  <dimension ref="A1:AC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC7" sqref="AC7"/>
+      <selection pane="bottomLeft" activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12425,7 +12428,7 @@
         <v>801</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
@@ -12442,7 +12445,7 @@
         <v>802</v>
       </c>
       <c r="E2" t="s">
-        <v>676</v>
+        <v>722</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -12451,13 +12454,13 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J2">
-        <v>0.32031900000000002</v>
+        <v>0.27889199999999997</v>
       </c>
       <c r="K2">
-        <v>2.1</v>
+        <v>2.5094400000000001</v>
       </c>
       <c r="L2">
         <v>0.1</v>
@@ -12484,7 +12487,7 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>6.3000600000000002</v>
+        <v>7.52841</v>
       </c>
       <c r="U2">
         <v>0.5</v>
@@ -12511,7 +12514,7 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -12528,7 +12531,7 @@
         <v>803</v>
       </c>
       <c r="E3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -12537,13 +12540,13 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J3">
-        <v>0.5</v>
+        <v>0.32031900000000002</v>
       </c>
       <c r="K3">
-        <v>2.50874</v>
+        <v>2.1</v>
       </c>
       <c r="L3">
         <v>0.1</v>
@@ -12570,7 +12573,7 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>7.5263</v>
+        <v>6.3000600000000002</v>
       </c>
       <c r="U3">
         <v>0.5</v>
@@ -12597,7 +12600,7 @@
         <v>0</v>
       </c>
       <c r="AC3">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -12614,7 +12617,7 @@
         <v>804</v>
       </c>
       <c r="E4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -12623,13 +12626,13 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J4">
         <v>0.5</v>
       </c>
       <c r="K4">
-        <v>3</v>
+        <v>2.50874</v>
       </c>
       <c r="L4">
         <v>0.1</v>
@@ -12656,7 +12659,7 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>9.0000900000000001</v>
+        <v>7.5263</v>
       </c>
       <c r="U4">
         <v>0.5</v>
@@ -12683,7 +12686,7 @@
         <v>0</v>
       </c>
       <c r="AC4">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -12700,7 +12703,7 @@
         <v>805</v>
       </c>
       <c r="E5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -12709,7 +12712,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J5">
         <v>0.5</v>
@@ -12769,7 +12772,7 @@
         <v>0</v>
       </c>
       <c r="AC5">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -12786,7 +12789,7 @@
         <v>806</v>
       </c>
       <c r="E6" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -12795,7 +12798,7 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J6">
         <v>0.5</v>
@@ -12855,7 +12858,7 @@
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -12872,7 +12875,7 @@
         <v>807</v>
       </c>
       <c r="E7" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -12887,7 +12890,7 @@
         <v>0.5</v>
       </c>
       <c r="K7">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="L7">
         <v>0.1</v>
@@ -12914,7 +12917,7 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>7</v>
+        <v>9.0000900000000001</v>
       </c>
       <c r="U7">
         <v>0.5</v>
@@ -12941,7 +12944,7 @@
         <v>0</v>
       </c>
       <c r="AC7">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -12958,7 +12961,7 @@
         <v>808</v>
       </c>
       <c r="E8" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -12967,10 +12970,10 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J8">
-        <v>0.29399199999999998</v>
+        <v>0.5</v>
       </c>
       <c r="K8">
         <v>2.1</v>
@@ -13027,7 +13030,7 @@
         <v>0</v>
       </c>
       <c r="AC8">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -13044,7 +13047,7 @@
         <v>809</v>
       </c>
       <c r="E9" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -13056,10 +13059,10 @@
         <v>20</v>
       </c>
       <c r="J9">
-        <v>0.385075</v>
+        <v>0.29399199999999998</v>
       </c>
       <c r="K9">
-        <v>3</v>
+        <v>2.1</v>
       </c>
       <c r="L9">
         <v>0.1</v>
@@ -13086,7 +13089,7 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>9.0000900000000001</v>
+        <v>7</v>
       </c>
       <c r="U9">
         <v>0.5</v>
@@ -13113,7 +13116,7 @@
         <v>0</v>
       </c>
       <c r="AC9">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -13130,7 +13133,7 @@
         <v>810</v>
       </c>
       <c r="E10" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -13142,7 +13145,7 @@
         <v>20</v>
       </c>
       <c r="J10">
-        <v>0.20569599999999999</v>
+        <v>0.385075</v>
       </c>
       <c r="K10">
         <v>3</v>
@@ -13199,7 +13202,7 @@
         <v>0</v>
       </c>
       <c r="AC10">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -13216,7 +13219,7 @@
         <v>811</v>
       </c>
       <c r="E11" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -13228,7 +13231,7 @@
         <v>20</v>
       </c>
       <c r="J11">
-        <v>0.41585</v>
+        <v>0.20569599999999999</v>
       </c>
       <c r="K11">
         <v>3</v>
@@ -13285,7 +13288,7 @@
         <v>0</v>
       </c>
       <c r="AC11">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -13302,7 +13305,7 @@
         <v>812</v>
       </c>
       <c r="E12" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -13314,7 +13317,7 @@
         <v>20</v>
       </c>
       <c r="J12">
-        <v>0.5</v>
+        <v>0.41585</v>
       </c>
       <c r="K12">
         <v>3</v>
@@ -13371,7 +13374,7 @@
         <v>0</v>
       </c>
       <c r="AC12">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
@@ -13388,7 +13391,7 @@
         <v>813</v>
       </c>
       <c r="E13" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -13457,7 +13460,7 @@
         <v>0</v>
       </c>
       <c r="AC13">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -13474,7 +13477,7 @@
         <v>814</v>
       </c>
       <c r="E14" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -13543,7 +13546,7 @@
         <v>0</v>
       </c>
       <c r="AC14">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -13560,7 +13563,7 @@
         <v>815</v>
       </c>
       <c r="E15" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -13575,7 +13578,7 @@
         <v>0.5</v>
       </c>
       <c r="K15">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="L15">
         <v>0.1</v>
@@ -13602,7 +13605,7 @@
         <v>0</v>
       </c>
       <c r="T15">
-        <v>6.3000600000000002</v>
+        <v>9.0000900000000001</v>
       </c>
       <c r="U15">
         <v>0.5</v>
@@ -13629,7 +13632,7 @@
         <v>0</v>
       </c>
       <c r="AC15">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
@@ -13646,7 +13649,7 @@
         <v>816</v>
       </c>
       <c r="E16" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -13661,7 +13664,7 @@
         <v>0.5</v>
       </c>
       <c r="K16">
-        <v>3</v>
+        <v>2.1</v>
       </c>
       <c r="L16">
         <v>0.1</v>
@@ -13688,7 +13691,7 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>9.0000900000000001</v>
+        <v>6.3000600000000002</v>
       </c>
       <c r="U16">
         <v>0.5</v>
@@ -13715,7 +13718,7 @@
         <v>0</v>
       </c>
       <c r="AC16">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -13732,7 +13735,7 @@
         <v>817</v>
       </c>
       <c r="E17" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -13744,10 +13747,10 @@
         <v>20</v>
       </c>
       <c r="J17">
-        <v>0.183088</v>
+        <v>0.5</v>
       </c>
       <c r="K17">
-        <v>0.51988800000000002</v>
+        <v>3</v>
       </c>
       <c r="L17">
         <v>0.1</v>
@@ -13774,7 +13777,7 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>1.55968</v>
+        <v>9.0000900000000001</v>
       </c>
       <c r="U17">
         <v>0.5</v>
@@ -13801,7 +13804,7 @@
         <v>0</v>
       </c>
       <c r="AC17">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
@@ -13818,7 +13821,7 @@
         <v>818</v>
       </c>
       <c r="E18" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -13830,10 +13833,10 @@
         <v>20</v>
       </c>
       <c r="J18">
-        <v>0.36373899999999998</v>
+        <v>0.183088</v>
       </c>
       <c r="K18">
-        <v>3</v>
+        <v>0.51988800000000002</v>
       </c>
       <c r="L18">
         <v>0.1</v>
@@ -13860,7 +13863,7 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <v>9.0000900000000001</v>
+        <v>1.55968</v>
       </c>
       <c r="U18">
         <v>0.5</v>
@@ -13887,7 +13890,7 @@
         <v>0</v>
       </c>
       <c r="AC18">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
@@ -13904,7 +13907,7 @@
         <v>819</v>
       </c>
       <c r="E19" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -13916,10 +13919,10 @@
         <v>20</v>
       </c>
       <c r="J19">
-        <v>0.5</v>
+        <v>0.36373899999999998</v>
       </c>
       <c r="K19">
-        <v>1.7178800000000001</v>
+        <v>3</v>
       </c>
       <c r="L19">
         <v>0.1</v>
@@ -13946,7 +13949,7 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>5.1536900000000001</v>
+        <v>9.0000900000000001</v>
       </c>
       <c r="U19">
         <v>0.5</v>
@@ -13973,7 +13976,7 @@
         <v>0</v>
       </c>
       <c r="AC19">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
@@ -13990,7 +13993,7 @@
         <v>820</v>
       </c>
       <c r="E20" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -14005,7 +14008,7 @@
         <v>0.5</v>
       </c>
       <c r="K20">
-        <v>0.71988200000000002</v>
+        <v>1.7178800000000001</v>
       </c>
       <c r="L20">
         <v>0.1</v>
@@ -14032,7 +14035,7 @@
         <v>0</v>
       </c>
       <c r="T20">
-        <v>2.39961</v>
+        <v>5.1536900000000001</v>
       </c>
       <c r="U20">
         <v>0.5</v>
@@ -14059,7 +14062,7 @@
         <v>0</v>
       </c>
       <c r="AC20">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
@@ -14076,7 +14079,7 @@
         <v>821</v>
       </c>
       <c r="E21" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -14085,13 +14088,13 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J21">
         <v>0.5</v>
       </c>
       <c r="K21">
-        <v>3</v>
+        <v>0.71988200000000002</v>
       </c>
       <c r="L21">
         <v>0.1</v>
@@ -14118,7 +14121,7 @@
         <v>0</v>
       </c>
       <c r="T21">
-        <v>9.0000900000000001</v>
+        <v>2.39961</v>
       </c>
       <c r="U21">
         <v>0.5</v>
@@ -14145,7 +14148,7 @@
         <v>0</v>
       </c>
       <c r="AC21">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
@@ -14162,7 +14165,7 @@
         <v>822</v>
       </c>
       <c r="E22" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -14171,13 +14174,13 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J22">
         <v>0.5</v>
       </c>
       <c r="K22">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="L22">
         <v>0.1</v>
@@ -14204,7 +14207,7 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>6.3000600000000002</v>
+        <v>9.0000900000000001</v>
       </c>
       <c r="U22">
         <v>0.5</v>
@@ -14231,7 +14234,7 @@
         <v>0</v>
       </c>
       <c r="AC22">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
@@ -14248,7 +14251,7 @@
         <v>823</v>
       </c>
       <c r="E23" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -14257,7 +14260,7 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J23">
         <v>0.5</v>
@@ -14290,7 +14293,7 @@
         <v>0</v>
       </c>
       <c r="T23">
-        <v>7</v>
+        <v>6.3000600000000002</v>
       </c>
       <c r="U23">
         <v>0.5</v>
@@ -14317,7 +14320,7 @@
         <v>0</v>
       </c>
       <c r="AC23">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
@@ -14334,7 +14337,7 @@
         <v>824</v>
       </c>
       <c r="E24" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -14343,13 +14346,13 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J24">
         <v>0.5</v>
       </c>
       <c r="K24">
-        <v>2.7096100000000001</v>
+        <v>2.1</v>
       </c>
       <c r="L24">
         <v>0.1</v>
@@ -14376,7 +14379,7 @@
         <v>0</v>
       </c>
       <c r="T24">
-        <v>8.1289099999999994</v>
+        <v>7</v>
       </c>
       <c r="U24">
         <v>0.5</v>
@@ -14403,7 +14406,7 @@
         <v>0</v>
       </c>
       <c r="AC24">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
@@ -14420,7 +14423,7 @@
         <v>825</v>
       </c>
       <c r="E25" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -14435,7 +14438,7 @@
         <v>0.5</v>
       </c>
       <c r="K25">
-        <v>3</v>
+        <v>2.7096100000000001</v>
       </c>
       <c r="L25">
         <v>0.1</v>
@@ -14462,7 +14465,7 @@
         <v>0</v>
       </c>
       <c r="T25">
-        <v>9.0000900000000001</v>
+        <v>8.1289099999999994</v>
       </c>
       <c r="U25">
         <v>0.5</v>
@@ -14489,7 +14492,7 @@
         <v>0</v>
       </c>
       <c r="AC25">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
@@ -14506,7 +14509,7 @@
         <v>826</v>
       </c>
       <c r="E26" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -14515,7 +14518,7 @@
         <v>1</v>
       </c>
       <c r="I26">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J26">
         <v>0.5</v>
@@ -14548,7 +14551,7 @@
         <v>0</v>
       </c>
       <c r="T26">
-        <v>10</v>
+        <v>9.0000900000000001</v>
       </c>
       <c r="U26">
         <v>0.5</v>
@@ -14575,7 +14578,93 @@
         <v>0</v>
       </c>
       <c r="AC26">
-        <v>200</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>827</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>827</v>
+      </c>
+      <c r="E27" t="s">
+        <v>721</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>25</v>
+      </c>
+      <c r="J27">
+        <v>0.5</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="L27">
+        <v>0.1</v>
+      </c>
+      <c r="M27">
+        <v>0.1</v>
+      </c>
+      <c r="N27">
+        <v>-0.1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0.4</v>
+      </c>
+      <c r="R27">
+        <v>0.5</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>10</v>
+      </c>
+      <c r="U27">
+        <v>0.5</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0.5</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0.05</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -14626,10 +14715,10 @@
         <v>730</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>731</v>
@@ -14649,13 +14738,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E2" t="s">
         <v>689</v>
@@ -14699,13 +14788,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="E3" t="s">
         <v>690</v>
@@ -14749,13 +14838,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="E4" t="s">
         <v>691</v>
@@ -14799,13 +14888,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E5" t="s">
         <v>692</v>
@@ -14849,13 +14938,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="E6" t="s">
         <v>693</v>
@@ -14899,13 +14988,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E7" t="s">
         <v>694</v>
@@ -14949,13 +15038,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="E8" t="s">
         <v>695</v>
@@ -14999,13 +15088,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="E9" t="s">
         <v>712</v>
@@ -15049,13 +15138,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="E10" t="s">
         <v>713</v>
@@ -15099,13 +15188,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="E11" t="s">
         <v>714</v>
@@ -15149,13 +15238,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E12" t="s">
         <v>715</v>
@@ -15199,13 +15288,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="E13" t="s">
         <v>716</v>
@@ -15249,13 +15338,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="E14" t="s">
         <v>717</v>
@@ -15299,13 +15388,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="E15" t="s">
         <v>718</v>
@@ -15349,13 +15438,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="E16" t="s">
         <v>719</v>
@@ -15399,13 +15488,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="E17" t="s">
         <v>723</v>
@@ -15449,13 +15538,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="E18" t="s">
         <v>724</v>
@@ -15527,22 +15616,22 @@
         <v>725</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>785</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -15550,13 +15639,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="E2" t="s">
         <v>676</v>
@@ -15585,13 +15674,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="E3" t="s">
         <v>677</v>
@@ -15620,13 +15709,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="E4" t="s">
         <v>678</v>
@@ -15655,13 +15744,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="E5" t="s">
         <v>679</v>
@@ -15690,13 +15779,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="E6" t="s">
         <v>680</v>
@@ -15725,13 +15814,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="E7" t="s">
         <v>681</v>
@@ -15760,13 +15849,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="E8" t="s">
         <v>682</v>
@@ -15795,13 +15884,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E9" t="s">
         <v>683</v>
@@ -15830,13 +15919,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="E10" t="s">
         <v>684</v>
@@ -15865,13 +15954,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="E11" t="s">
         <v>685</v>
@@ -15900,13 +15989,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="E12" t="s">
         <v>686</v>
@@ -15935,13 +16024,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="E13" t="s">
         <v>687</v>
@@ -15970,13 +16059,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="E14" t="s">
         <v>688</v>
@@ -16005,13 +16094,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="E15" t="s">
         <v>689</v>
@@ -16040,13 +16129,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E16" t="s">
         <v>690</v>
@@ -16075,13 +16164,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="E17" t="s">
         <v>691</v>
@@ -16110,13 +16199,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="E18" t="s">
         <v>692</v>
@@ -16145,13 +16234,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="E19" t="s">
         <v>693</v>
@@ -16180,13 +16269,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E20" t="s">
         <v>694</v>
@@ -16215,13 +16304,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="E21" t="s">
         <v>695</v>
@@ -16250,13 +16339,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="E22" t="s">
         <v>696</v>
@@ -16285,13 +16374,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="E23" t="s">
         <v>697</v>
@@ -16320,13 +16409,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="E24" t="s">
         <v>698</v>
@@ -16355,13 +16444,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="E25" t="s">
         <v>699</v>
@@ -16390,13 +16479,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="E26" t="s">
         <v>700</v>
@@ -16425,13 +16514,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="E27" t="s">
         <v>701</v>
@@ -16460,13 +16549,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="E28" t="s">
         <v>702</v>
@@ -16495,13 +16584,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="E29" t="s">
         <v>703</v>
@@ -16530,13 +16619,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="E30" t="s">
         <v>704</v>
@@ -16565,13 +16654,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="E31" t="s">
         <v>705</v>
@@ -16600,13 +16689,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C32">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="E32" t="s">
         <v>706</v>
@@ -16635,13 +16724,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="E33" t="s">
         <v>707</v>
@@ -16670,13 +16759,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="E34" t="s">
         <v>708</v>
@@ -16705,13 +16794,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="E35" t="s">
         <v>709</v>
@@ -16740,13 +16829,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="E36" t="s">
         <v>710</v>
@@ -16775,13 +16864,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="E37" t="s">
         <v>711</v>
@@ -16810,13 +16899,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="E38" t="s">
         <v>712</v>
@@ -16845,13 +16934,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="E39" t="s">
         <v>713</v>
@@ -16880,13 +16969,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="E40" t="s">
         <v>714</v>
@@ -16915,13 +17004,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="E41" t="s">
         <v>715</v>
@@ -16950,13 +17039,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="E42" t="s">
         <v>716</v>
@@ -16985,13 +17074,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="E43" t="s">
         <v>717</v>
@@ -17020,13 +17109,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="E44" t="s">
         <v>718</v>
@@ -17055,13 +17144,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="E45" t="s">
         <v>719</v>
@@ -17090,13 +17179,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E46" t="s">
         <v>720</v>
@@ -17125,13 +17214,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E47" t="s">
         <v>721</v>
@@ -17160,13 +17249,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="E48" t="s">
         <v>722</v>
@@ -17195,13 +17284,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="E49" t="s">
         <v>723</v>
@@ -17230,13 +17319,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E50" t="s">
         <v>724</v>
@@ -17267,16 +17356,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y1" sqref="Y1:Y7"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -17299,49 +17388,49 @@
         <v>377</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>665</v>
@@ -17349,20 +17438,19 @@
       <c r="X1" s="1" t="s">
         <v>666</v>
       </c>
-      <c r="Y1" s="2"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="E2">
         <v>65</v>
@@ -17425,18 +17513,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="E3">
         <v>104</v>
@@ -17499,18 +17587,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="E4">
         <v>105</v>
@@ -17573,18 +17661,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="E5">
         <v>114</v>
@@ -17647,18 +17735,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="E6">
         <v>115</v>
@@ -17721,18 +17809,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="E7">
         <v>147</v>
@@ -17825,70 +17913,70 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>378</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>729</v>
@@ -17897,28 +17985,28 @@
         <v>730</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>788</v>
@@ -17927,58 +18015,58 @@
         <v>789</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.2">
@@ -17986,16 +18074,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="E2" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -18153,16 +18241,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="E3" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -18320,16 +18408,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="E4" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -18487,16 +18575,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="E5" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -18654,16 +18742,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="E6" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -18821,16 +18909,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="E7" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -19013,109 +19101,109 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>378</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
@@ -19123,16 +19211,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="E2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="F2" t="s">
         <v>595</v>
@@ -19230,16 +19318,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="E3" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="F3" t="s">
         <v>615</v>
@@ -19337,16 +19425,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E4" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="F4" t="s">
         <v>616</v>
@@ -19444,16 +19532,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E5" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="F5" t="s">
         <v>618</v>
@@ -19551,16 +19639,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="E6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="F6" t="s">
         <v>619</v>
@@ -19658,16 +19746,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="E7" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="F7" t="s">
         <v>630</v>
@@ -19790,16 +19878,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>657</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -19807,16 +19895,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="E2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -19833,16 +19921,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E3" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -19859,16 +19947,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="E4" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -19885,16 +19973,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="E5" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -19911,16 +19999,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="E6" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -19937,16 +20025,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E7" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -48412,7 +48500,7 @@
         <v>691</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>691</v>
@@ -48501,7 +48589,7 @@
         <v>692</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
         <v>692</v>
@@ -48768,7 +48856,7 @@
         <v>695</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>695</v>
@@ -50281,7 +50369,7 @@
         <v>712</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
         <v>712</v>
@@ -50370,7 +50458,7 @@
         <v>713</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
         <v>713</v>
@@ -50459,7 +50547,7 @@
         <v>714</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
         <v>714</v>
@@ -50548,7 +50636,7 @@
         <v>715</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
         <v>715</v>
@@ -50726,7 +50814,7 @@
         <v>717</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
         <v>717</v>
@@ -50815,7 +50903,7 @@
         <v>718</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
         <v>718</v>
@@ -51260,7 +51348,7 @@
         <v>723</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
         <v>723</v>
@@ -51349,7 +51437,7 @@
         <v>724</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
         <v>724</v>
@@ -51440,7 +51528,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -53522,7 +53610,7 @@
         <v>781</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>781</v>

</xml_diff>